<commit_message>
feat: update plan xmind and plan table
</commit_message>
<xml_diff>
--- a/___/table/Two thousand and twenty-two/2022 Year calendar-almanac_monthly_plan.xlsx
+++ b/___/table/Two thousand and twenty-two/2022 Year calendar-almanac_monthly_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="667"/>
+    <workbookView windowWidth="24225" windowHeight="12540" tabRatio="667" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="年历" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <numFmt numFmtId="177" formatCode="0&quot;年&quot;"/>
     <numFmt numFmtId="178" formatCode="mmmm"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +183,13 @@
       <b/>
       <sz val="12"/>
       <color theme="4" tint="-0.25"/>
+      <name val="汉仪君黑-45简"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
       <name val="汉仪君黑-45简"/>
       <charset val="134"/>
     </font>
@@ -399,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="51">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +427,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,10 +949,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -942,40 +961,37 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="23" fillId="5" borderId="0">
+    <xf numFmtId="176" fontId="24" fillId="7" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -987,98 +1003,101 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="27" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="29" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="29" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="30" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1124,104 +1143,116 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="16" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="6" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="8" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="12" applyFont="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="12" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="5" borderId="0" xfId="9" applyFont="1">
+    <xf numFmtId="176" fontId="20" fillId="7" borderId="0" xfId="9" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="7" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="9" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="8" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="10" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="9" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="11" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="10" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="12" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="11" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="13" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="12" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="14" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="13" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="15" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="14" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="16" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="15" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="17" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="16" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="18" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="17" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="18" fillId="19" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -7842,1977 +7873,1977 @@
   <sheetPr/>
   <dimension ref="A2:AH26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="26" customWidth="1"/>
-    <col min="2" max="2" width="3.625" style="26" customWidth="1"/>
-    <col min="3" max="33" width="4.75" style="26" customWidth="1"/>
-    <col min="34" max="34" width="3.625" style="26" customWidth="1"/>
-    <col min="35" max="35" width="3" style="26" customWidth="1"/>
-    <col min="36" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="3.25" style="30" customWidth="1"/>
+    <col min="2" max="2" width="3.625" style="30" customWidth="1"/>
+    <col min="3" max="33" width="4.75" style="30" customWidth="1"/>
+    <col min="34" max="34" width="3.625" style="30" customWidth="1"/>
+    <col min="35" max="35" width="3" style="30" customWidth="1"/>
+    <col min="36" max="16384" width="9" style="30"/>
   </cols>
   <sheetData>
     <row r="2" ht="72" customHeight="1" spans="1:34">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="51"/>
-    </row>
-    <row r="3" s="25" customFormat="1" ht="22" customHeight="1" spans="2:34">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32" t="s">
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="55"/>
+    </row>
+    <row r="3" s="29" customFormat="1" ht="22" customHeight="1" spans="2:34">
+      <c r="B3" s="35"/>
+      <c r="C3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="41" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="40"/>
-      <c r="S3" s="45" t="s">
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="40"/>
-      <c r="AA3" s="48" t="s">
+      <c r="T3" s="49"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="44"/>
+      <c r="AA3" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="AB3" s="48"/>
-      <c r="AC3" s="48"/>
-      <c r="AD3" s="48"/>
-      <c r="AE3" s="48"/>
-      <c r="AF3" s="48"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="52"/>
+      <c r="AB3" s="52"/>
+      <c r="AC3" s="52"/>
+      <c r="AD3" s="52"/>
+      <c r="AE3" s="52"/>
+      <c r="AF3" s="52"/>
+      <c r="AG3" s="52"/>
+      <c r="AH3" s="56"/>
     </row>
     <row r="4" ht="20" customHeight="1" spans="2:34">
-      <c r="B4" s="33"/>
-      <c r="C4" s="34" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="34" t="s">
+      <c r="L4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="34" t="s">
+      <c r="M4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="34" t="s">
+      <c r="N4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="34" t="s">
+      <c r="P4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="34" t="s">
+      <c r="Q4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="34" t="s">
+      <c r="S4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="34" t="s">
+      <c r="T4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="34" t="s">
+      <c r="U4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="V4" s="34" t="s">
+      <c r="V4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="W4" s="34" t="s">
+      <c r="W4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="X4" s="34" t="s">
+      <c r="X4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="34" t="s">
+      <c r="Y4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AA4" s="34" t="s">
+      <c r="AA4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AB4" s="34" t="s">
+      <c r="AB4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AC4" s="34" t="s">
+      <c r="AC4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="34" t="s">
+      <c r="AD4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AE4" s="34" t="s">
+      <c r="AE4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AF4" s="34" t="s">
+      <c r="AF4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AG4" s="34" t="s">
+      <c r="AG4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AH4" s="53"/>
+      <c r="AH4" s="57"/>
     </row>
     <row r="5" ht="20" customHeight="1" spans="2:34">
-      <c r="B5" s="33"/>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="35">
+      <c r="F5" s="39">
         <v>43831</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="39">
         <v>43832</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="39">
         <v>43833</v>
       </c>
-      <c r="I5" s="35">
+      <c r="I5" s="39">
         <v>43834</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="35" t="s">
+      <c r="L5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="M5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="35" t="s">
+      <c r="O5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="35" t="s">
+      <c r="P5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="39">
         <v>43862</v>
       </c>
-      <c r="S5" s="35">
+      <c r="S5" s="39">
         <v>43891</v>
       </c>
-      <c r="T5" s="35">
+      <c r="T5" s="39">
         <v>43892</v>
       </c>
-      <c r="U5" s="35">
+      <c r="U5" s="39">
         <v>43893</v>
       </c>
-      <c r="V5" s="35">
+      <c r="V5" s="39">
         <v>43894</v>
       </c>
-      <c r="W5" s="35">
+      <c r="W5" s="39">
         <v>43895</v>
       </c>
-      <c r="X5" s="35">
+      <c r="X5" s="39">
         <v>43896</v>
       </c>
-      <c r="Y5" s="35">
+      <c r="Y5" s="39">
         <v>43897</v>
       </c>
-      <c r="AA5" s="35" t="s">
+      <c r="AA5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="35" t="s">
+      <c r="AB5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AC5" s="35" t="s">
+      <c r="AC5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AD5" s="35">
+      <c r="AD5" s="39">
         <v>43922</v>
       </c>
-      <c r="AE5" s="35">
+      <c r="AE5" s="39">
         <v>43923</v>
       </c>
-      <c r="AF5" s="35">
+      <c r="AF5" s="39">
         <v>43924</v>
       </c>
-      <c r="AG5" s="35">
+      <c r="AG5" s="39">
         <v>43925</v>
       </c>
-      <c r="AH5" s="53"/>
+      <c r="AH5" s="57"/>
     </row>
     <row r="6" ht="20" customHeight="1" spans="2:34">
-      <c r="B6" s="33"/>
-      <c r="C6" s="35">
+      <c r="B6" s="37"/>
+      <c r="C6" s="39">
         <v>43835</v>
       </c>
-      <c r="D6" s="35">
+      <c r="D6" s="39">
         <v>43836</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="39">
         <v>43837</v>
       </c>
-      <c r="F6" s="35">
+      <c r="F6" s="39">
         <v>43838</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="39">
         <v>43839</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="39">
         <v>43840</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="39">
         <v>43841</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="39">
         <v>43863</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="39">
         <v>43864</v>
       </c>
-      <c r="M6" s="35">
+      <c r="M6" s="39">
         <v>43865</v>
       </c>
-      <c r="N6" s="35">
+      <c r="N6" s="39">
         <v>43866</v>
       </c>
-      <c r="O6" s="35">
+      <c r="O6" s="39">
         <v>43867</v>
       </c>
-      <c r="P6" s="35">
+      <c r="P6" s="39">
         <v>43868</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="39">
         <v>43869</v>
       </c>
-      <c r="S6" s="35">
+      <c r="S6" s="39">
         <v>43898</v>
       </c>
-      <c r="T6" s="35">
+      <c r="T6" s="39">
         <v>43899</v>
       </c>
-      <c r="U6" s="35">
+      <c r="U6" s="39">
         <v>43900</v>
       </c>
-      <c r="V6" s="35">
+      <c r="V6" s="39">
         <v>43901</v>
       </c>
-      <c r="W6" s="35">
+      <c r="W6" s="39">
         <v>43902</v>
       </c>
-      <c r="X6" s="35">
+      <c r="X6" s="39">
         <v>43903</v>
       </c>
-      <c r="Y6" s="35">
+      <c r="Y6" s="39">
         <v>43904</v>
       </c>
-      <c r="AA6" s="35">
+      <c r="AA6" s="39">
         <v>43926</v>
       </c>
-      <c r="AB6" s="35">
+      <c r="AB6" s="39">
         <v>43927</v>
       </c>
-      <c r="AC6" s="35">
+      <c r="AC6" s="39">
         <v>43928</v>
       </c>
-      <c r="AD6" s="35">
+      <c r="AD6" s="39">
         <v>43929</v>
       </c>
-      <c r="AE6" s="35">
+      <c r="AE6" s="39">
         <v>43930</v>
       </c>
-      <c r="AF6" s="35">
+      <c r="AF6" s="39">
         <v>43931</v>
       </c>
-      <c r="AG6" s="35">
+      <c r="AG6" s="39">
         <v>43932</v>
       </c>
-      <c r="AH6" s="53"/>
+      <c r="AH6" s="57"/>
     </row>
     <row r="7" ht="20" customHeight="1" spans="2:34">
-      <c r="B7" s="33"/>
-      <c r="C7" s="35">
+      <c r="B7" s="37"/>
+      <c r="C7" s="39">
         <v>43842</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="39">
         <v>43843</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="39">
         <v>43844</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="39">
         <v>43845</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="39">
         <v>43846</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="39">
         <v>43847</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="39">
         <v>43848</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="39">
         <v>43870</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="39">
         <v>43871</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="39">
         <v>43872</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="39">
         <v>43873</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="39">
         <v>43874</v>
       </c>
-      <c r="P7" s="35">
+      <c r="P7" s="39">
         <v>43875</v>
       </c>
-      <c r="Q7" s="35">
+      <c r="Q7" s="39">
         <v>43876</v>
       </c>
-      <c r="S7" s="35">
+      <c r="S7" s="39">
         <v>43905</v>
       </c>
-      <c r="T7" s="35">
+      <c r="T7" s="39">
         <v>43906</v>
       </c>
-      <c r="U7" s="35">
+      <c r="U7" s="39">
         <v>43907</v>
       </c>
-      <c r="V7" s="35">
+      <c r="V7" s="39">
         <v>43908</v>
       </c>
-      <c r="W7" s="35">
+      <c r="W7" s="39">
         <v>43909</v>
       </c>
-      <c r="X7" s="35">
+      <c r="X7" s="39">
         <v>43910</v>
       </c>
-      <c r="Y7" s="35">
+      <c r="Y7" s="39">
         <v>43911</v>
       </c>
-      <c r="AA7" s="35">
+      <c r="AA7" s="39">
         <v>43933</v>
       </c>
-      <c r="AB7" s="35">
+      <c r="AB7" s="39">
         <v>43934</v>
       </c>
-      <c r="AC7" s="35">
+      <c r="AC7" s="39">
         <v>43935</v>
       </c>
-      <c r="AD7" s="35">
+      <c r="AD7" s="39">
         <v>43936</v>
       </c>
-      <c r="AE7" s="35">
+      <c r="AE7" s="39">
         <v>43937</v>
       </c>
-      <c r="AF7" s="35">
+      <c r="AF7" s="39">
         <v>43938</v>
       </c>
-      <c r="AG7" s="35">
+      <c r="AG7" s="39">
         <v>43939</v>
       </c>
-      <c r="AH7" s="53"/>
+      <c r="AH7" s="57"/>
     </row>
     <row r="8" ht="20" customHeight="1" spans="2:34">
-      <c r="B8" s="33"/>
-      <c r="C8" s="35">
+      <c r="B8" s="37"/>
+      <c r="C8" s="39">
         <v>43849</v>
       </c>
-      <c r="D8" s="35">
+      <c r="D8" s="39">
         <v>43850</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="39">
         <v>43851</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="39">
         <v>43852</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="39">
         <v>43853</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="39">
         <v>43854</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="39">
         <v>43855</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="39">
         <v>43877</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="39">
         <v>43878</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="39">
         <v>43879</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="39">
         <v>43880</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="39">
         <v>43881</v>
       </c>
-      <c r="P8" s="35">
+      <c r="P8" s="39">
         <v>43882</v>
       </c>
-      <c r="Q8" s="35">
+      <c r="Q8" s="39">
         <v>43883</v>
       </c>
-      <c r="S8" s="35">
+      <c r="S8" s="39">
         <v>43912</v>
       </c>
-      <c r="T8" s="35">
+      <c r="T8" s="39">
         <v>43913</v>
       </c>
-      <c r="U8" s="35">
+      <c r="U8" s="39">
         <v>43914</v>
       </c>
-      <c r="V8" s="35">
+      <c r="V8" s="39">
         <v>43915</v>
       </c>
-      <c r="W8" s="35">
+      <c r="W8" s="39">
         <v>43916</v>
       </c>
-      <c r="X8" s="35">
+      <c r="X8" s="39">
         <v>43917</v>
       </c>
-      <c r="Y8" s="35">
+      <c r="Y8" s="39">
         <v>43918</v>
       </c>
-      <c r="AA8" s="35">
+      <c r="AA8" s="39">
         <v>43940</v>
       </c>
-      <c r="AB8" s="35">
+      <c r="AB8" s="39">
         <v>43941</v>
       </c>
-      <c r="AC8" s="35">
+      <c r="AC8" s="39">
         <v>43942</v>
       </c>
-      <c r="AD8" s="35">
+      <c r="AD8" s="39">
         <v>43943</v>
       </c>
-      <c r="AE8" s="35">
+      <c r="AE8" s="39">
         <v>43944</v>
       </c>
-      <c r="AF8" s="35">
+      <c r="AF8" s="39">
         <v>43945</v>
       </c>
-      <c r="AG8" s="35">
+      <c r="AG8" s="39">
         <v>43946</v>
       </c>
-      <c r="AH8" s="53"/>
+      <c r="AH8" s="57"/>
     </row>
     <row r="9" ht="20" customHeight="1" spans="2:34">
-      <c r="B9" s="33"/>
-      <c r="C9" s="35">
+      <c r="B9" s="37"/>
+      <c r="C9" s="39">
         <v>43856</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="39">
         <v>43857</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="39">
         <v>43858</v>
       </c>
-      <c r="F9" s="35">
+      <c r="F9" s="39">
         <v>43859</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="39">
         <v>43860</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="39">
         <v>43861</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="39">
         <v>43884</v>
       </c>
-      <c r="L9" s="35">
+      <c r="L9" s="39">
         <v>43885</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="39">
         <v>43886</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="39">
         <v>43887</v>
       </c>
-      <c r="O9" s="35">
+      <c r="O9" s="39">
         <v>43888</v>
       </c>
-      <c r="P9" s="35">
+      <c r="P9" s="39">
         <v>43889</v>
       </c>
-      <c r="Q9" s="35"/>
-      <c r="S9" s="35">
+      <c r="Q9" s="39"/>
+      <c r="S9" s="39">
         <v>43919</v>
       </c>
-      <c r="T9" s="35">
+      <c r="T9" s="39">
         <v>43920</v>
       </c>
-      <c r="U9" s="35">
+      <c r="U9" s="39">
         <v>43921</v>
       </c>
-      <c r="V9" s="35" t="s">
+      <c r="V9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="W9" s="35" t="s">
+      <c r="W9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="X9" s="35" t="s">
+      <c r="X9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Y9" s="35" t="s">
+      <c r="Y9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AA9" s="35">
+      <c r="AA9" s="39">
         <v>43947</v>
       </c>
-      <c r="AB9" s="35">
+      <c r="AB9" s="39">
         <v>43948</v>
       </c>
-      <c r="AC9" s="35">
+      <c r="AC9" s="39">
         <v>43949</v>
       </c>
-      <c r="AD9" s="35">
+      <c r="AD9" s="39">
         <v>43950</v>
       </c>
-      <c r="AE9" s="35">
+      <c r="AE9" s="39">
         <v>43951</v>
       </c>
-      <c r="AF9" s="35" t="s">
+      <c r="AF9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AG9" s="35" t="s">
+      <c r="AG9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AH9" s="53"/>
+      <c r="AH9" s="57"/>
     </row>
     <row r="10" ht="20" customHeight="1" spans="2:34">
-      <c r="B10" s="33"/>
-      <c r="C10" s="35" t="s">
+      <c r="B10" s="37"/>
+      <c r="C10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="35" t="s">
+      <c r="K10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="35" t="s">
+      <c r="L10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="M10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="35" t="s">
+      <c r="N10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="O10" s="35" t="s">
+      <c r="O10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="P10" s="35" t="s">
+      <c r="P10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q10" s="35" t="s">
+      <c r="Q10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="S10" s="35" t="s">
+      <c r="S10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="35" t="s">
+      <c r="T10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="35" t="s">
+      <c r="U10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="V10" s="35" t="s">
+      <c r="V10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="W10" s="35" t="s">
+      <c r="W10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="X10" s="35" t="s">
+      <c r="X10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Y10" s="35" t="s">
+      <c r="Y10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AA10" s="35" t="s">
+      <c r="AA10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AB10" s="35" t="s">
+      <c r="AB10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AC10" s="35" t="s">
+      <c r="AC10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AD10" s="35" t="s">
+      <c r="AD10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AE10" s="35" t="s">
+      <c r="AE10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AF10" s="35" t="s">
+      <c r="AF10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AG10" s="35" t="s">
+      <c r="AG10" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AH10" s="53"/>
-    </row>
-    <row r="11" s="25" customFormat="1" ht="22" customHeight="1" spans="2:34">
-      <c r="B11" s="31"/>
-      <c r="C11" s="36" t="s">
+      <c r="AH10" s="57"/>
+    </row>
+    <row r="11" s="29" customFormat="1" ht="22" customHeight="1" spans="2:34">
+      <c r="B11" s="35"/>
+      <c r="C11" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="43" t="s">
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="L11" s="43"/>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="46" t="s">
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="46"/>
-      <c r="W11" s="46"/>
-      <c r="X11" s="46"/>
-      <c r="Y11" s="46"/>
-      <c r="Z11" s="42"/>
-      <c r="AA11" s="49" t="s">
+      <c r="T11" s="50"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="46"/>
+      <c r="AA11" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="AB11" s="49"/>
-      <c r="AC11" s="49"/>
-      <c r="AD11" s="49"/>
-      <c r="AE11" s="49"/>
-      <c r="AF11" s="49"/>
-      <c r="AG11" s="49"/>
-      <c r="AH11" s="52"/>
+      <c r="AB11" s="53"/>
+      <c r="AC11" s="53"/>
+      <c r="AD11" s="53"/>
+      <c r="AE11" s="53"/>
+      <c r="AF11" s="53"/>
+      <c r="AG11" s="53"/>
+      <c r="AH11" s="56"/>
     </row>
     <row r="12" ht="20" customHeight="1" spans="2:34">
-      <c r="B12" s="33"/>
-      <c r="C12" s="34" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="34" t="s">
+      <c r="G12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="34" t="s">
+      <c r="L12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="34" t="s">
+      <c r="M12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="N12" s="34" t="s">
+      <c r="N12" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="O12" s="34" t="s">
+      <c r="O12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="P12" s="34" t="s">
+      <c r="P12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q12" s="34" t="s">
+      <c r="Q12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="S12" s="34" t="s">
+      <c r="S12" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="T12" s="34" t="s">
+      <c r="T12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="U12" s="34" t="s">
+      <c r="U12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="V12" s="34" t="s">
+      <c r="V12" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="W12" s="34" t="s">
+      <c r="W12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="X12" s="34" t="s">
+      <c r="X12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Y12" s="34" t="s">
+      <c r="Y12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AA12" s="34" t="s">
+      <c r="AA12" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AB12" s="34" t="s">
+      <c r="AB12" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AC12" s="34" t="s">
+      <c r="AC12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AD12" s="34" t="s">
+      <c r="AD12" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AE12" s="34" t="s">
+      <c r="AE12" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AF12" s="34" t="s">
+      <c r="AF12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AG12" s="34" t="s">
+      <c r="AG12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AH12" s="53"/>
+      <c r="AH12" s="57"/>
     </row>
     <row r="13" ht="20" customHeight="1" spans="2:34">
-      <c r="B13" s="33"/>
-      <c r="C13" s="35" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="39">
         <v>43952</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="39">
         <v>43953</v>
       </c>
-      <c r="K13" s="35" t="s">
+      <c r="K13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="35">
+      <c r="L13" s="39">
         <v>43983</v>
       </c>
-      <c r="M13" s="35">
+      <c r="M13" s="39">
         <v>43984</v>
       </c>
-      <c r="N13" s="35">
+      <c r="N13" s="39">
         <v>43985</v>
       </c>
-      <c r="O13" s="35">
+      <c r="O13" s="39">
         <v>43986</v>
       </c>
-      <c r="P13" s="35">
+      <c r="P13" s="39">
         <v>43987</v>
       </c>
-      <c r="Q13" s="35">
+      <c r="Q13" s="39">
         <v>43988</v>
       </c>
-      <c r="S13" s="35" t="s">
+      <c r="S13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="T13" s="35" t="s">
+      <c r="T13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="U13" s="35" t="s">
+      <c r="U13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="V13" s="35">
+      <c r="V13" s="39">
         <v>44013</v>
       </c>
-      <c r="W13" s="35">
+      <c r="W13" s="39">
         <v>44014</v>
       </c>
-      <c r="X13" s="35">
+      <c r="X13" s="39">
         <v>44015</v>
       </c>
-      <c r="Y13" s="35">
+      <c r="Y13" s="39">
         <v>44016</v>
       </c>
-      <c r="AA13" s="35" t="s">
+      <c r="AA13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AB13" s="35" t="s">
+      <c r="AB13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AC13" s="35" t="s">
+      <c r="AC13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AD13" s="35" t="s">
+      <c r="AD13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AE13" s="35" t="s">
+      <c r="AE13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AF13" s="35" t="s">
+      <c r="AF13" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AG13" s="35">
+      <c r="AG13" s="39">
         <v>44044</v>
       </c>
-      <c r="AH13" s="53"/>
+      <c r="AH13" s="57"/>
     </row>
     <row r="14" ht="20" customHeight="1" spans="2:34">
-      <c r="B14" s="33"/>
-      <c r="C14" s="35">
+      <c r="B14" s="37"/>
+      <c r="C14" s="39">
         <v>43954</v>
       </c>
-      <c r="D14" s="35">
+      <c r="D14" s="39">
         <v>43955</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="39">
         <v>43956</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="39">
         <v>43957</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G14" s="39">
         <v>43958</v>
       </c>
-      <c r="H14" s="35">
+      <c r="H14" s="39">
         <v>43959</v>
       </c>
-      <c r="I14" s="35">
+      <c r="I14" s="39">
         <v>43960</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="39">
         <v>43989</v>
       </c>
-      <c r="L14" s="35">
+      <c r="L14" s="39">
         <v>43990</v>
       </c>
-      <c r="M14" s="35">
+      <c r="M14" s="39">
         <v>43991</v>
       </c>
-      <c r="N14" s="35">
+      <c r="N14" s="39">
         <v>43992</v>
       </c>
-      <c r="O14" s="35">
+      <c r="O14" s="39">
         <v>43993</v>
       </c>
-      <c r="P14" s="35">
+      <c r="P14" s="39">
         <v>43994</v>
       </c>
-      <c r="Q14" s="35">
+      <c r="Q14" s="39">
         <v>43995</v>
       </c>
-      <c r="S14" s="35">
+      <c r="S14" s="39">
         <v>44017</v>
       </c>
-      <c r="T14" s="35">
+      <c r="T14" s="39">
         <v>44018</v>
       </c>
-      <c r="U14" s="35">
+      <c r="U14" s="39">
         <v>44019</v>
       </c>
-      <c r="V14" s="35">
+      <c r="V14" s="39">
         <v>44020</v>
       </c>
-      <c r="W14" s="35">
+      <c r="W14" s="39">
         <v>44021</v>
       </c>
-      <c r="X14" s="35">
+      <c r="X14" s="39">
         <v>44022</v>
       </c>
-      <c r="Y14" s="35">
+      <c r="Y14" s="39">
         <v>44023</v>
       </c>
-      <c r="AA14" s="35">
+      <c r="AA14" s="39">
         <v>44045</v>
       </c>
-      <c r="AB14" s="35">
+      <c r="AB14" s="39">
         <v>44046</v>
       </c>
-      <c r="AC14" s="35">
+      <c r="AC14" s="39">
         <v>44047</v>
       </c>
-      <c r="AD14" s="35">
+      <c r="AD14" s="39">
         <v>44048</v>
       </c>
-      <c r="AE14" s="35">
+      <c r="AE14" s="39">
         <v>44049</v>
       </c>
-      <c r="AF14" s="35">
+      <c r="AF14" s="39">
         <v>44050</v>
       </c>
-      <c r="AG14" s="35">
+      <c r="AG14" s="39">
         <v>44051</v>
       </c>
-      <c r="AH14" s="53"/>
+      <c r="AH14" s="57"/>
     </row>
     <row r="15" ht="20" customHeight="1" spans="2:34">
-      <c r="B15" s="33"/>
-      <c r="C15" s="35">
+      <c r="B15" s="37"/>
+      <c r="C15" s="39">
         <v>43961</v>
       </c>
-      <c r="D15" s="35">
+      <c r="D15" s="39">
         <v>43962</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="39">
         <v>43963</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="39">
         <v>43964</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="39">
         <v>43965</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H15" s="39">
         <v>43966</v>
       </c>
-      <c r="I15" s="35">
+      <c r="I15" s="39">
         <v>43967</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K15" s="39">
         <v>43996</v>
       </c>
-      <c r="L15" s="35">
+      <c r="L15" s="39">
         <v>43997</v>
       </c>
-      <c r="M15" s="35">
+      <c r="M15" s="39">
         <v>43998</v>
       </c>
-      <c r="N15" s="35">
+      <c r="N15" s="39">
         <v>43999</v>
       </c>
-      <c r="O15" s="35">
+      <c r="O15" s="39">
         <v>44000</v>
       </c>
-      <c r="P15" s="35">
+      <c r="P15" s="39">
         <v>44001</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q15" s="39">
         <v>44002</v>
       </c>
-      <c r="S15" s="35">
+      <c r="S15" s="39">
         <v>44024</v>
       </c>
-      <c r="T15" s="35">
+      <c r="T15" s="39">
         <v>44025</v>
       </c>
-      <c r="U15" s="35">
+      <c r="U15" s="39">
         <v>44026</v>
       </c>
-      <c r="V15" s="35">
+      <c r="V15" s="39">
         <v>44027</v>
       </c>
-      <c r="W15" s="35">
+      <c r="W15" s="39">
         <v>44028</v>
       </c>
-      <c r="X15" s="35">
+      <c r="X15" s="39">
         <v>44029</v>
       </c>
-      <c r="Y15" s="35">
+      <c r="Y15" s="39">
         <v>44030</v>
       </c>
-      <c r="AA15" s="35">
+      <c r="AA15" s="39">
         <v>44052</v>
       </c>
-      <c r="AB15" s="35">
+      <c r="AB15" s="39">
         <v>44053</v>
       </c>
-      <c r="AC15" s="35">
+      <c r="AC15" s="39">
         <v>44054</v>
       </c>
-      <c r="AD15" s="35">
+      <c r="AD15" s="39">
         <v>44055</v>
       </c>
-      <c r="AE15" s="35">
+      <c r="AE15" s="39">
         <v>44056</v>
       </c>
-      <c r="AF15" s="35">
+      <c r="AF15" s="39">
         <v>44057</v>
       </c>
-      <c r="AG15" s="35">
+      <c r="AG15" s="39">
         <v>44058</v>
       </c>
-      <c r="AH15" s="53"/>
+      <c r="AH15" s="57"/>
     </row>
     <row r="16" ht="20" customHeight="1" spans="2:34">
-      <c r="B16" s="33"/>
-      <c r="C16" s="35">
+      <c r="B16" s="37"/>
+      <c r="C16" s="39">
         <v>43968</v>
       </c>
-      <c r="D16" s="35">
+      <c r="D16" s="39">
         <v>43969</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="39">
         <v>43970</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="39">
         <v>43971</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G16" s="39">
         <v>43972</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H16" s="39">
         <v>43973</v>
       </c>
-      <c r="I16" s="35">
+      <c r="I16" s="39">
         <v>43974</v>
       </c>
-      <c r="K16" s="35">
+      <c r="K16" s="39">
         <v>44003</v>
       </c>
-      <c r="L16" s="35">
+      <c r="L16" s="39">
         <v>44004</v>
       </c>
-      <c r="M16" s="35">
+      <c r="M16" s="39">
         <v>44005</v>
       </c>
-      <c r="N16" s="35">
+      <c r="N16" s="39">
         <v>44006</v>
       </c>
-      <c r="O16" s="35">
+      <c r="O16" s="39">
         <v>44007</v>
       </c>
-      <c r="P16" s="35">
+      <c r="P16" s="39">
         <v>44008</v>
       </c>
-      <c r="Q16" s="35">
+      <c r="Q16" s="39">
         <v>44009</v>
       </c>
-      <c r="S16" s="35">
+      <c r="S16" s="39">
         <v>44031</v>
       </c>
-      <c r="T16" s="35">
+      <c r="T16" s="39">
         <v>44032</v>
       </c>
-      <c r="U16" s="35">
+      <c r="U16" s="39">
         <v>44033</v>
       </c>
-      <c r="V16" s="35">
+      <c r="V16" s="39">
         <v>44034</v>
       </c>
-      <c r="W16" s="35">
+      <c r="W16" s="39">
         <v>44035</v>
       </c>
-      <c r="X16" s="35">
+      <c r="X16" s="39">
         <v>44036</v>
       </c>
-      <c r="Y16" s="35">
+      <c r="Y16" s="39">
         <v>44037</v>
       </c>
-      <c r="AA16" s="35">
+      <c r="AA16" s="39">
         <v>44059</v>
       </c>
-      <c r="AB16" s="35">
+      <c r="AB16" s="39">
         <v>44060</v>
       </c>
-      <c r="AC16" s="35">
+      <c r="AC16" s="39">
         <v>44061</v>
       </c>
-      <c r="AD16" s="35">
+      <c r="AD16" s="39">
         <v>44062</v>
       </c>
-      <c r="AE16" s="35">
+      <c r="AE16" s="39">
         <v>44063</v>
       </c>
-      <c r="AF16" s="35">
+      <c r="AF16" s="39">
         <v>44064</v>
       </c>
-      <c r="AG16" s="35">
+      <c r="AG16" s="39">
         <v>44065</v>
       </c>
-      <c r="AH16" s="53"/>
+      <c r="AH16" s="57"/>
     </row>
     <row r="17" ht="20" customHeight="1" spans="2:34">
-      <c r="B17" s="33"/>
-      <c r="C17" s="35">
+      <c r="B17" s="37"/>
+      <c r="C17" s="39">
         <v>43975</v>
       </c>
-      <c r="D17" s="35">
+      <c r="D17" s="39">
         <v>43976</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="39">
         <v>43977</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="39">
         <v>43978</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="39">
         <v>43979</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="39">
         <v>43980</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="39">
         <v>43981</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="39">
         <v>44010</v>
       </c>
-      <c r="L17" s="35">
+      <c r="L17" s="39">
         <v>44011</v>
       </c>
-      <c r="M17" s="35">
+      <c r="M17" s="39">
         <v>44012</v>
       </c>
-      <c r="N17" s="35" t="s">
+      <c r="N17" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="P17" s="35" t="s">
+      <c r="P17" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q17" s="35" t="s">
+      <c r="Q17" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="S17" s="35">
+      <c r="S17" s="39">
         <v>44038</v>
       </c>
-      <c r="T17" s="35">
+      <c r="T17" s="39">
         <v>44039</v>
       </c>
-      <c r="U17" s="35">
+      <c r="U17" s="39">
         <v>44040</v>
       </c>
-      <c r="V17" s="35">
+      <c r="V17" s="39">
         <v>44041</v>
       </c>
-      <c r="W17" s="35">
+      <c r="W17" s="39">
         <v>44042</v>
       </c>
-      <c r="X17" s="35">
+      <c r="X17" s="39">
         <v>44043</v>
       </c>
-      <c r="Y17" s="35" t="s">
+      <c r="Y17" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AA17" s="35">
+      <c r="AA17" s="39">
         <v>44066</v>
       </c>
-      <c r="AB17" s="35">
+      <c r="AB17" s="39">
         <v>44067</v>
       </c>
-      <c r="AC17" s="35">
+      <c r="AC17" s="39">
         <v>44068</v>
       </c>
-      <c r="AD17" s="35">
+      <c r="AD17" s="39">
         <v>44069</v>
       </c>
-      <c r="AE17" s="35">
+      <c r="AE17" s="39">
         <v>44070</v>
       </c>
-      <c r="AF17" s="35">
+      <c r="AF17" s="39">
         <v>44071</v>
       </c>
-      <c r="AG17" s="35">
+      <c r="AG17" s="39">
         <v>44072</v>
       </c>
-      <c r="AH17" s="53"/>
+      <c r="AH17" s="57"/>
     </row>
     <row r="18" ht="20" customHeight="1" spans="2:34">
-      <c r="B18" s="33"/>
-      <c r="C18" s="35">
+      <c r="B18" s="37"/>
+      <c r="C18" s="39">
         <v>43982</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="35" t="s">
+      <c r="I18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K18" s="35" t="s">
+      <c r="K18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L18" s="35" t="s">
+      <c r="L18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M18" s="35" t="s">
+      <c r="M18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="35" t="s">
+      <c r="N18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="35" t="s">
+      <c r="O18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="P18" s="35" t="s">
+      <c r="P18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q18" s="35" t="s">
+      <c r="Q18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="S18" s="35" t="s">
+      <c r="S18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="T18" s="35" t="s">
+      <c r="T18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="U18" s="35" t="s">
+      <c r="U18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="V18" s="35" t="s">
+      <c r="V18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="W18" s="35" t="s">
+      <c r="W18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="X18" s="35" t="s">
+      <c r="X18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Y18" s="35" t="s">
+      <c r="Y18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AA18" s="35">
+      <c r="AA18" s="39">
         <v>44073</v>
       </c>
-      <c r="AB18" s="35">
+      <c r="AB18" s="39">
         <v>44074</v>
       </c>
-      <c r="AC18" s="35" t="s">
+      <c r="AC18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AD18" s="35" t="s">
+      <c r="AD18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AE18" s="35" t="s">
+      <c r="AE18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AF18" s="35" t="s">
+      <c r="AF18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AG18" s="35" t="s">
+      <c r="AG18" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AH18" s="53"/>
-    </row>
-    <row r="19" s="25" customFormat="1" ht="22" customHeight="1" spans="2:34">
-      <c r="B19" s="31"/>
-      <c r="C19" s="37" t="s">
+      <c r="AH18" s="57"/>
+    </row>
+    <row r="19" s="29" customFormat="1" ht="22" customHeight="1" spans="2:34">
+      <c r="B19" s="35"/>
+      <c r="C19" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="44" t="s">
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="47" t="s">
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="T19" s="47"/>
-      <c r="U19" s="47"/>
-      <c r="V19" s="47"/>
-      <c r="W19" s="47"/>
-      <c r="X19" s="47"/>
-      <c r="Y19" s="47"/>
-      <c r="Z19" s="42"/>
-      <c r="AA19" s="50" t="s">
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="46"/>
+      <c r="AA19" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="AB19" s="50"/>
-      <c r="AC19" s="50"/>
-      <c r="AD19" s="50"/>
-      <c r="AE19" s="50"/>
-      <c r="AF19" s="50"/>
-      <c r="AG19" s="50"/>
-      <c r="AH19" s="52"/>
+      <c r="AB19" s="54"/>
+      <c r="AC19" s="54"/>
+      <c r="AD19" s="54"/>
+      <c r="AE19" s="54"/>
+      <c r="AF19" s="54"/>
+      <c r="AG19" s="54"/>
+      <c r="AH19" s="56"/>
     </row>
     <row r="20" ht="20" customHeight="1" spans="2:34">
-      <c r="B20" s="33"/>
-      <c r="C20" s="34" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="E20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="G20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="K20" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="L20" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="34" t="s">
+      <c r="M20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="N20" s="34" t="s">
+      <c r="N20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="O20" s="34" t="s">
+      <c r="O20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="P20" s="34" t="s">
+      <c r="P20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Q20" s="34" t="s">
+      <c r="Q20" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="S20" s="34" t="s">
+      <c r="S20" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="T20" s="34" t="s">
+      <c r="T20" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="U20" s="34" t="s">
+      <c r="U20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="V20" s="34" t="s">
+      <c r="V20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="W20" s="34" t="s">
+      <c r="W20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="X20" s="34" t="s">
+      <c r="X20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="Y20" s="34" t="s">
+      <c r="Y20" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AA20" s="34" t="s">
+      <c r="AA20" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AB20" s="34" t="s">
+      <c r="AB20" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AC20" s="34" t="s">
+      <c r="AC20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AD20" s="34" t="s">
+      <c r="AD20" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="AE20" s="34" t="s">
+      <c r="AE20" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="AF20" s="34" t="s">
+      <c r="AF20" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AG20" s="34" t="s">
+      <c r="AG20" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AH20" s="53"/>
+      <c r="AH20" s="57"/>
     </row>
     <row r="21" ht="20" customHeight="1" spans="2:34">
-      <c r="B21" s="33"/>
-      <c r="C21" s="35" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="39">
         <v>44075</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="39">
         <v>44076</v>
       </c>
-      <c r="G21" s="35">
+      <c r="G21" s="39">
         <v>44077</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="39">
         <v>44078</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="39">
         <v>44079</v>
       </c>
-      <c r="K21" s="35" t="s">
+      <c r="K21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="35" t="s">
+      <c r="L21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M21" s="35" t="s">
+      <c r="M21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="N21" s="35" t="s">
+      <c r="N21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="39">
         <v>44105</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P21" s="39">
         <v>44106</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="39">
         <v>44107</v>
       </c>
-      <c r="S21" s="35">
+      <c r="S21" s="39">
         <v>44136</v>
       </c>
-      <c r="T21" s="35">
+      <c r="T21" s="39">
         <v>44137</v>
       </c>
-      <c r="U21" s="35">
+      <c r="U21" s="39">
         <v>44138</v>
       </c>
-      <c r="V21" s="35">
+      <c r="V21" s="39">
         <v>44139</v>
       </c>
-      <c r="W21" s="35">
+      <c r="W21" s="39">
         <v>44140</v>
       </c>
-      <c r="X21" s="35">
+      <c r="X21" s="39">
         <v>44141</v>
       </c>
-      <c r="Y21" s="35">
+      <c r="Y21" s="39">
         <v>44142</v>
       </c>
-      <c r="AA21" s="35" t="s">
+      <c r="AA21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AB21" s="35" t="s">
+      <c r="AB21" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AC21" s="35">
+      <c r="AC21" s="39">
         <v>44166</v>
       </c>
-      <c r="AD21" s="35">
+      <c r="AD21" s="39">
         <v>44167</v>
       </c>
-      <c r="AE21" s="35">
+      <c r="AE21" s="39">
         <v>44168</v>
       </c>
-      <c r="AF21" s="35">
+      <c r="AF21" s="39">
         <v>44169</v>
       </c>
-      <c r="AG21" s="35">
+      <c r="AG21" s="39">
         <v>44170</v>
       </c>
-      <c r="AH21" s="53"/>
+      <c r="AH21" s="57"/>
     </row>
     <row r="22" ht="20" customHeight="1" spans="2:34">
-      <c r="B22" s="33"/>
-      <c r="C22" s="35">
+      <c r="B22" s="37"/>
+      <c r="C22" s="39">
         <v>44080</v>
       </c>
-      <c r="D22" s="35">
+      <c r="D22" s="39">
         <v>44081</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="39">
         <v>44082</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="39">
         <v>44083</v>
       </c>
-      <c r="G22" s="35">
+      <c r="G22" s="39">
         <v>44084</v>
       </c>
-      <c r="H22" s="35">
+      <c r="H22" s="39">
         <v>44085</v>
       </c>
-      <c r="I22" s="35">
+      <c r="I22" s="39">
         <v>44086</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="39">
         <v>44108</v>
       </c>
-      <c r="L22" s="35">
+      <c r="L22" s="39">
         <v>44109</v>
       </c>
-      <c r="M22" s="35">
+      <c r="M22" s="39">
         <v>44110</v>
       </c>
-      <c r="N22" s="35">
+      <c r="N22" s="39">
         <v>44111</v>
       </c>
-      <c r="O22" s="35">
+      <c r="O22" s="39">
         <v>44112</v>
       </c>
-      <c r="P22" s="35">
+      <c r="P22" s="39">
         <v>44113</v>
       </c>
-      <c r="Q22" s="35">
+      <c r="Q22" s="39">
         <v>44114</v>
       </c>
-      <c r="S22" s="35">
+      <c r="S22" s="39">
         <v>44143</v>
       </c>
-      <c r="T22" s="35">
+      <c r="T22" s="39">
         <v>44144</v>
       </c>
-      <c r="U22" s="35">
+      <c r="U22" s="39">
         <v>44145</v>
       </c>
-      <c r="V22" s="35">
+      <c r="V22" s="39">
         <v>44146</v>
       </c>
-      <c r="W22" s="35">
+      <c r="W22" s="39">
         <v>44147</v>
       </c>
-      <c r="X22" s="35">
+      <c r="X22" s="39">
         <v>44148</v>
       </c>
-      <c r="Y22" s="35">
+      <c r="Y22" s="39">
         <v>44149</v>
       </c>
-      <c r="AA22" s="35">
+      <c r="AA22" s="39">
         <v>44171</v>
       </c>
-      <c r="AB22" s="35">
+      <c r="AB22" s="39">
         <v>44172</v>
       </c>
-      <c r="AC22" s="35">
+      <c r="AC22" s="39">
         <v>44173</v>
       </c>
-      <c r="AD22" s="35">
+      <c r="AD22" s="39">
         <v>44174</v>
       </c>
-      <c r="AE22" s="35">
+      <c r="AE22" s="39">
         <v>44175</v>
       </c>
-      <c r="AF22" s="35">
+      <c r="AF22" s="39">
         <v>44176</v>
       </c>
-      <c r="AG22" s="35">
+      <c r="AG22" s="39">
         <v>44177</v>
       </c>
-      <c r="AH22" s="53"/>
+      <c r="AH22" s="57"/>
     </row>
     <row r="23" ht="20" customHeight="1" spans="2:34">
-      <c r="B23" s="33"/>
-      <c r="C23" s="35">
+      <c r="B23" s="37"/>
+      <c r="C23" s="39">
         <v>44087</v>
       </c>
-      <c r="D23" s="35">
+      <c r="D23" s="39">
         <v>44088</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="39">
         <v>44089</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="39">
         <v>44090</v>
       </c>
-      <c r="G23" s="35">
+      <c r="G23" s="39">
         <v>44091</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H23" s="39">
         <v>44092</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I23" s="39">
         <v>44093</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="39">
         <v>44115</v>
       </c>
-      <c r="L23" s="35">
+      <c r="L23" s="39">
         <v>44116</v>
       </c>
-      <c r="M23" s="35">
+      <c r="M23" s="39">
         <v>44117</v>
       </c>
-      <c r="N23" s="35">
+      <c r="N23" s="39">
         <v>44118</v>
       </c>
-      <c r="O23" s="35">
+      <c r="O23" s="39">
         <v>44119</v>
       </c>
-      <c r="P23" s="35">
+      <c r="P23" s="39">
         <v>44120</v>
       </c>
-      <c r="Q23" s="35">
+      <c r="Q23" s="39">
         <v>44121</v>
       </c>
-      <c r="S23" s="35">
+      <c r="S23" s="39">
         <v>44150</v>
       </c>
-      <c r="T23" s="35">
+      <c r="T23" s="39">
         <v>44151</v>
       </c>
-      <c r="U23" s="35">
+      <c r="U23" s="39">
         <v>44152</v>
       </c>
-      <c r="V23" s="35">
+      <c r="V23" s="39">
         <v>44153</v>
       </c>
-      <c r="W23" s="35">
+      <c r="W23" s="39">
         <v>44154</v>
       </c>
-      <c r="X23" s="35">
+      <c r="X23" s="39">
         <v>44155</v>
       </c>
-      <c r="Y23" s="35">
+      <c r="Y23" s="39">
         <v>44156</v>
       </c>
-      <c r="AA23" s="35">
+      <c r="AA23" s="39">
         <v>44178</v>
       </c>
-      <c r="AB23" s="35">
+      <c r="AB23" s="39">
         <v>44179</v>
       </c>
-      <c r="AC23" s="35">
+      <c r="AC23" s="39">
         <v>44180</v>
       </c>
-      <c r="AD23" s="35">
+      <c r="AD23" s="39">
         <v>44181</v>
       </c>
-      <c r="AE23" s="35">
+      <c r="AE23" s="39">
         <v>44182</v>
       </c>
-      <c r="AF23" s="35">
+      <c r="AF23" s="39">
         <v>44183</v>
       </c>
-      <c r="AG23" s="35">
+      <c r="AG23" s="39">
         <v>44184</v>
       </c>
-      <c r="AH23" s="53"/>
+      <c r="AH23" s="57"/>
     </row>
     <row r="24" ht="20" customHeight="1" spans="2:34">
-      <c r="B24" s="33"/>
-      <c r="C24" s="35">
+      <c r="B24" s="37"/>
+      <c r="C24" s="39">
         <v>44094</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="39">
         <v>44095</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="39">
         <v>44096</v>
       </c>
-      <c r="F24" s="35">
+      <c r="F24" s="39">
         <v>44097</v>
       </c>
-      <c r="G24" s="35">
+      <c r="G24" s="39">
         <v>44098</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H24" s="39">
         <v>44099</v>
       </c>
-      <c r="I24" s="35">
+      <c r="I24" s="39">
         <v>44100</v>
       </c>
-      <c r="K24" s="35">
+      <c r="K24" s="39">
         <v>44122</v>
       </c>
-      <c r="L24" s="35">
+      <c r="L24" s="39">
         <v>44123</v>
       </c>
-      <c r="M24" s="35">
+      <c r="M24" s="39">
         <v>44124</v>
       </c>
-      <c r="N24" s="35">
+      <c r="N24" s="39">
         <v>44125</v>
       </c>
-      <c r="O24" s="35">
+      <c r="O24" s="39">
         <v>44126</v>
       </c>
-      <c r="P24" s="35">
+      <c r="P24" s="39">
         <v>44127</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="39">
         <v>44128</v>
       </c>
-      <c r="S24" s="35">
+      <c r="S24" s="39">
         <v>44157</v>
       </c>
-      <c r="T24" s="35">
+      <c r="T24" s="39">
         <v>44158</v>
       </c>
-      <c r="U24" s="35">
+      <c r="U24" s="39">
         <v>44159</v>
       </c>
-      <c r="V24" s="35">
+      <c r="V24" s="39">
         <v>44160</v>
       </c>
-      <c r="W24" s="35">
+      <c r="W24" s="39">
         <v>44161</v>
       </c>
-      <c r="X24" s="35">
+      <c r="X24" s="39">
         <v>44162</v>
       </c>
-      <c r="Y24" s="35">
+      <c r="Y24" s="39">
         <v>44163</v>
       </c>
-      <c r="AA24" s="35">
+      <c r="AA24" s="39">
         <v>44185</v>
       </c>
-      <c r="AB24" s="35">
+      <c r="AB24" s="39">
         <v>44186</v>
       </c>
-      <c r="AC24" s="35">
+      <c r="AC24" s="39">
         <v>44187</v>
       </c>
-      <c r="AD24" s="35">
+      <c r="AD24" s="39">
         <v>44188</v>
       </c>
-      <c r="AE24" s="35">
+      <c r="AE24" s="39">
         <v>44189</v>
       </c>
-      <c r="AF24" s="35">
+      <c r="AF24" s="39">
         <v>44190</v>
       </c>
-      <c r="AG24" s="35">
+      <c r="AG24" s="39">
         <v>44191</v>
       </c>
-      <c r="AH24" s="53"/>
+      <c r="AH24" s="57"/>
     </row>
     <row r="25" ht="20" customHeight="1" spans="2:34">
-      <c r="B25" s="33"/>
-      <c r="C25" s="35">
+      <c r="B25" s="37"/>
+      <c r="C25" s="39">
         <v>44101</v>
       </c>
-      <c r="D25" s="35">
+      <c r="D25" s="39">
         <v>44102</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="39">
         <v>44103</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="39">
         <v>44104</v>
       </c>
-      <c r="G25" s="35" t="s">
+      <c r="G25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="I25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K25" s="35">
+      <c r="K25" s="39">
         <v>44129</v>
       </c>
-      <c r="L25" s="35">
+      <c r="L25" s="39">
         <v>44130</v>
       </c>
-      <c r="M25" s="35">
+      <c r="M25" s="39">
         <v>44131</v>
       </c>
-      <c r="N25" s="35">
+      <c r="N25" s="39">
         <v>44132</v>
       </c>
-      <c r="O25" s="35">
+      <c r="O25" s="39">
         <v>44133</v>
       </c>
-      <c r="P25" s="35">
+      <c r="P25" s="39">
         <v>44134</v>
       </c>
-      <c r="Q25" s="35">
+      <c r="Q25" s="39">
         <v>44135</v>
       </c>
-      <c r="S25" s="35">
+      <c r="S25" s="39">
         <v>44164</v>
       </c>
-      <c r="T25" s="35">
+      <c r="T25" s="39">
         <v>44165</v>
       </c>
-      <c r="U25" s="35" t="s">
+      <c r="U25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="V25" s="35" t="s">
+      <c r="V25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="W25" s="35" t="s">
+      <c r="W25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="X25" s="35" t="s">
+      <c r="X25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Y25" s="35" t="s">
+      <c r="Y25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AA25" s="35">
+      <c r="AA25" s="39">
         <v>44192</v>
       </c>
-      <c r="AB25" s="35">
+      <c r="AB25" s="39">
         <v>44193</v>
       </c>
-      <c r="AC25" s="35">
+      <c r="AC25" s="39">
         <v>44194</v>
       </c>
-      <c r="AD25" s="35">
+      <c r="AD25" s="39">
         <v>44195</v>
       </c>
-      <c r="AE25" s="35">
+      <c r="AE25" s="39">
         <v>44196</v>
       </c>
-      <c r="AF25" s="35" t="s">
+      <c r="AF25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AG25" s="35" t="s">
+      <c r="AG25" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AH25" s="53"/>
+      <c r="AH25" s="57"/>
     </row>
     <row r="26" ht="45" customHeight="1" spans="2:34">
-      <c r="B26" s="38"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="39"/>
-      <c r="R26" s="39"/>
-      <c r="S26" s="39"/>
-      <c r="T26" s="39"/>
-      <c r="U26" s="39"/>
-      <c r="V26" s="39"/>
-      <c r="W26" s="39"/>
-      <c r="X26" s="39"/>
-      <c r="Y26" s="39"/>
-      <c r="Z26" s="39"/>
-      <c r="AA26" s="39"/>
-      <c r="AB26" s="39"/>
-      <c r="AC26" s="39"/>
-      <c r="AD26" s="39"/>
-      <c r="AE26" s="39"/>
-      <c r="AF26" s="39"/>
-      <c r="AG26" s="39"/>
-      <c r="AH26" s="54"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="43"/>
+      <c r="T26" s="43"/>
+      <c r="U26" s="43"/>
+      <c r="V26" s="43"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="43"/>
+      <c r="Y26" s="43"/>
+      <c r="Z26" s="43"/>
+      <c r="AA26" s="43"/>
+      <c r="AB26" s="43"/>
+      <c r="AC26" s="43"/>
+      <c r="AD26" s="43"/>
+      <c r="AE26" s="43"/>
+      <c r="AF26" s="43"/>
+      <c r="AG26" s="43"/>
+      <c r="AH26" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -10295,8 +10326,8 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20" customHeight="1"/>
@@ -10389,7 +10420,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="14"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" customHeight="1" spans="2:9">
       <c r="B7" s="7"/>
@@ -10419,12 +10450,12 @@
       <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="14"/>
     </row>
     <row r="9" customHeight="1" spans="2:9">
@@ -10495,7 +10526,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" customHeight="1" spans="2:9">
       <c r="B13" s="7"/>
@@ -10525,7 +10556,7 @@
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -10830,7 +10861,7 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="14"/>
+      <c r="I6" s="15"/>
     </row>
     <row r="7" customHeight="1" spans="2:9">
       <c r="B7" s="7"/>
@@ -11618,17 +11649,17 @@
   <sheetPr/>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="19.875" style="18" customWidth="1"/>
-    <col min="3" max="6" width="19.875" style="19" customWidth="1"/>
-    <col min="7" max="9" width="19.875" style="20" customWidth="1"/>
-    <col min="10" max="16384" width="10" style="18"/>
+    <col min="1" max="1" width="3.375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="19.875" style="22" customWidth="1"/>
+    <col min="3" max="6" width="19.875" style="23" customWidth="1"/>
+    <col min="7" max="9" width="19.875" style="24" customWidth="1"/>
+    <col min="10" max="16384" width="10" style="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="18" customHeight="1"/>
@@ -11656,8 +11687,8 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" s="17" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A4" s="21"/>
+    <row r="4" s="21" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A4" s="25"/>
       <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
@@ -11683,8 +11714,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" s="17" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A5" s="21"/>
+    <row r="5" s="21" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A5" s="25"/>
       <c r="B5" s="7"/>
       <c r="C5" s="9">
         <v>25</v>
@@ -11708,19 +11739,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" s="17" customFormat="1" ht="65" customHeight="1" spans="1:9">
-      <c r="A6" s="21"/>
+    <row r="6" s="21" customFormat="1" ht="65" customHeight="1" spans="1:9">
+      <c r="A6" s="25"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" s="17" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A7" s="21"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="26"/>
+    </row>
+    <row r="7" s="21" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A7" s="25"/>
       <c r="B7" s="7"/>
       <c r="C7" s="13">
         <v>2</v>
@@ -11744,21 +11775,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" s="17" customFormat="1" ht="65" customHeight="1" spans="1:9">
-      <c r="A8" s="21"/>
+    <row r="8" s="21" customFormat="1" ht="65" customHeight="1" spans="1:9">
+      <c r="A8" s="25"/>
       <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="22"/>
-    </row>
-    <row r="9" s="17" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A9" s="21"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="26"/>
+    </row>
+    <row r="9" s="21" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A9" s="25"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13">
         <v>9</v>
@@ -11782,19 +11813,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" s="17" customFormat="1" ht="65" customHeight="1" spans="1:9">
-      <c r="A10" s="21"/>
+    <row r="10" s="21" customFormat="1" ht="65" customHeight="1" spans="1:9">
+      <c r="A10" s="25"/>
       <c r="B10" s="7"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="22"/>
-    </row>
-    <row r="11" s="17" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A11" s="21"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" s="21" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A11" s="25"/>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
@@ -11820,19 +11851,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" s="17" customFormat="1" ht="65" customHeight="1" spans="1:9">
-      <c r="A12" s="21"/>
+    <row r="12" s="21" customFormat="1" ht="65" customHeight="1" spans="1:9">
+      <c r="A12" s="25"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" s="17" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A13" s="21"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="26"/>
+    </row>
+    <row r="13" s="21" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A13" s="25"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13">
         <v>23</v>
@@ -11856,21 +11887,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" s="17" customFormat="1" ht="65" customHeight="1" spans="1:9">
-      <c r="A14" s="21"/>
+    <row r="14" s="21" customFormat="1" ht="65" customHeight="1" spans="1:9">
+      <c r="A14" s="25"/>
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" s="17" customFormat="1" customHeight="1" spans="1:9">
-      <c r="A15" s="21"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" s="21" customFormat="1" customHeight="1" spans="1:9">
+      <c r="A15" s="25"/>
       <c r="B15" s="7"/>
       <c r="C15" s="13">
         <v>30</v>
@@ -11894,16 +11925,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" s="17" customFormat="1" ht="65" customHeight="1" spans="1:9">
-      <c r="A16" s="21"/>
+    <row r="16" s="21" customFormat="1" ht="65" customHeight="1" spans="1:9">
+      <c r="A16" s="25"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="22"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -12165,10 +12196,10 @@
       <c r="B6" s="7"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
       <c r="I6" s="14"/>
     </row>
     <row r="7" customHeight="1" spans="2:9">
@@ -12305,8 +12336,8 @@
       <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -13933,7 +13964,7 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="15"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" customHeight="1" spans="2:9">
       <c r="B7" s="7"/>
@@ -13969,7 +14000,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" customHeight="1" spans="2:9">
       <c r="B9" s="7"/>
@@ -14003,7 +14034,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" customHeight="1" spans="2:9">
       <c r="B11" s="7" t="s">
@@ -14039,7 +14070,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="15"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" customHeight="1" spans="2:9">
       <c r="B13" s="7"/>
@@ -14368,13 +14399,13 @@
     </row>
     <row r="6" ht="65" customHeight="1" spans="2:9">
       <c r="B6" s="7"/>
-      <c r="C6" s="15"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="15"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" customHeight="1" spans="2:9">
       <c r="B7" s="7"/>
@@ -14410,7 +14441,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" customHeight="1" spans="2:9">
       <c r="B9" s="7"/>
@@ -14444,7 +14475,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" customHeight="1" spans="2:9">
       <c r="B11" s="7" t="s">
@@ -14480,7 +14511,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="15"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" customHeight="1" spans="2:9">
       <c r="B13" s="7"/>
@@ -14516,7 +14547,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" customHeight="1" spans="2:9">
       <c r="B15" s="7"/>
@@ -14809,13 +14840,13 @@
     </row>
     <row r="6" ht="65" customHeight="1" spans="2:9">
       <c r="B6" s="7"/>
-      <c r="C6" s="15"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="I6" s="15"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" customHeight="1" spans="2:9">
       <c r="B7" s="7"/>
@@ -14851,7 +14882,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
-      <c r="I8" s="15"/>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" customHeight="1" spans="2:9">
       <c r="B9" s="7"/>
@@ -14885,7 +14916,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="15"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" customHeight="1" spans="2:9">
       <c r="B11" s="7" t="s">
@@ -14921,7 +14952,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
-      <c r="I12" s="15"/>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" customHeight="1" spans="2:9">
       <c r="B13" s="7"/>
@@ -14985,10 +15016,10 @@
     </row>
     <row r="16" ht="65" customHeight="1" spans="2:9">
       <c r="B16" s="7"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>

</xml_diff>

<commit_message>
feat: update gantt table
</commit_message>
<xml_diff>
--- a/___/table/Two thousand and twenty-two/2022 Year calendar-almanac_monthly_plan.xlsx
+++ b/___/table/Two thousand and twenty-two/2022 Year calendar-almanac_monthly_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540" tabRatio="667" activeTab="10"/>
+    <workbookView windowWidth="28125" windowHeight="12540" tabRatio="667" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="年历" sheetId="1" r:id="rId1"/>
@@ -10327,7 +10327,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="20" customHeight="1"/>

</xml_diff>